<commit_message>
succesfull integration and csv format
</commit_message>
<xml_diff>
--- a/Sven/Meteorological_Data.xlsx
+++ b/Sven/Meteorological_Data.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">Date Time </t>
+    <t xml:space="preserve">Date Time</t>
   </si>
   <si>
     <t xml:space="preserve">Wind Direction</t>
   </si>
   <si>
-    <t xml:space="preserve">Wind Speed (m/s)</t>
+    <t xml:space="preserve">Wind Speed</t>
   </si>
   <si>
     <t xml:space="preserve">Elevation (m)</t>
@@ -149,14 +149,14 @@
   <dimension ref="A1:E708"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>